<commit_message>
Add "out of" to "Advanced Stats"
</commit_message>
<xml_diff>
--- a/2019_topps-update_odds.xlsx
+++ b/2019_topps-update_odds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aadams/Library/Mobile Documents/com~apple~CloudDocs/baseball-card/2019_topps-update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aadams/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5E1411-AB64-CA4F-9C05-7FD5DD690ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C211197-1210-3644-9DF1-4BD38FF655C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="460" windowWidth="36400" windowHeight="27240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,9 +282,9 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="#,##0;;\–"/>
-    <numFmt numFmtId="169" formatCode="&quot;1:&quot;0.0"/>
+    <numFmt numFmtId="166" formatCode="&quot;1:&quot;0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -325,6 +325,11 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -354,7 +359,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
@@ -408,7 +413,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -418,21 +423,35 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="25">
     <dxf>
-      <numFmt numFmtId="169" formatCode="&quot;1:&quot;0.0"/>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF0F7FD"/>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -452,6 +471,60 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF0F7FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF0F7FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="&quot;1:&quot;0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF0F7FD"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -483,32 +556,6 @@
         <b/>
         <family val="2"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF0F7FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF0F7FD"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -763,9 +810,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{2FC81C60-A550-524B-A41C-3D95C6355A37}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstColumn" dxfId="18"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="firstColumn" dxfId="22"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -859,26 +906,26 @@
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{DA8F3C11-F8FD-2C4E-908A-4EB9FB8EFCCB}" name="CardType" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{6E8EA256-F14A-4449-B3C6-45F5155D8E6A}" name="Variation"/>
-    <tableColumn id="4" xr3:uid="{ACBF3844-63C8-F449-A249-7D13D59F04AE}" name="IsHit" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{ACBF3844-63C8-F449-A249-7D13D59F04AE}" name="IsHit" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{DDDE1690-C6E2-C641-B4E9-571C0D1D8680}" name="NumberedTo"/>
-    <tableColumn id="16" xr3:uid="{4793CECF-D483-5C4D-841C-5DEB3D049282}" name="JumboOdds" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{C706747D-6E8F-B942-B312-1D6369EEB544}" name="HobbyOdds" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{FFB92347-880C-8443-99A1-FC976C15DCEB}" name="HangerOdds" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{0B3903E7-EDAA-CF48-8698-90E8CC0DA792}" name="FatOdds" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{785CD13C-5A26-BC4C-8977-9BEDE08204F4}" name="BlasterOdds" dataDxfId="12"/>
-    <tableColumn id="17" xr3:uid="{E4A8AE1A-CD17-4843-9E8A-A6D5CB612C56}" name="JumboNorm" dataDxfId="11">
+    <tableColumn id="16" xr3:uid="{4793CECF-D483-5C4D-841C-5DEB3D049282}" name="JumboOdds" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{C706747D-6E8F-B942-B312-1D6369EEB544}" name="HobbyOdds" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{FFB92347-880C-8443-99A1-FC976C15DCEB}" name="HangerOdds" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{0B3903E7-EDAA-CF48-8698-90E8CC0DA792}" name="FatOdds" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{785CD13C-5A26-BC4C-8977-9BEDE08204F4}" name="BlasterOdds" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{E4A8AE1A-CD17-4843-9E8A-A6D5CB612C56}" name="JumboNorm" dataDxfId="15">
       <calculatedColumnFormula>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[JumboOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[JumboOdds]],0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{BE2B76D6-249B-B242-97E2-8468BB7E3DB4}" name="HobbyNorm" dataDxfId="10">
+    <tableColumn id="20" xr3:uid="{BE2B76D6-249B-B242-97E2-8468BB7E3DB4}" name="HobbyNorm" dataDxfId="14">
       <calculatedColumnFormula>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HobbyOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HobbyOdds]],0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4E2BDC61-7D8C-5448-8BC9-CFD89D45B2F3}" name="HangerNorm" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{4E2BDC61-7D8C-5448-8BC9-CFD89D45B2F3}" name="HangerNorm" dataDxfId="13">
       <calculatedColumnFormula>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HangerOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HangerOdds]],0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{11A3CC37-C28B-B842-B274-AE9EE82A811B}" name="FatNorm" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{11A3CC37-C28B-B842-B274-AE9EE82A811B}" name="FatNorm" dataDxfId="12">
       <calculatedColumnFormula>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[FatOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[FatOdds]],0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{52D57D7C-8849-5847-8773-21A27BDDA278}" name="BlasterNorm" dataDxfId="7">
+    <tableColumn id="11" xr3:uid="{52D57D7C-8849-5847-8773-21A27BDDA278}" name="BlasterNorm" dataDxfId="11">
       <calculatedColumnFormula>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[BlasterOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[BlasterOdds]],0),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -889,14 +936,14 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67438B45-4855-0A4B-9E14-8405D347D3A4}" name="HitsPerBox" displayName="HitsPerBox" ref="A1:G6" totalsRowShown="0">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF3D4B4D-B221-9146-BF3E-0A1712EF0EA9}" name="Product" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{AF3D4B4D-B221-9146-BF3E-0A1712EF0EA9}" name="Product" dataDxfId="10"/>
     <tableColumn id="8" xr3:uid="{188F180E-8836-E748-B12C-F3F55ACCA3F1}" name="Packs/Box"/>
     <tableColumn id="7" xr3:uid="{FE16E6AD-07FA-5E41-A145-567C508A5E18}" name="Price/Box" dataCellStyle="Currency"/>
-    <tableColumn id="11" xr3:uid="{9F620024-2BED-494E-9163-1FC07C6150B3}" name="Price/Pack" dataDxfId="3" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{9F620024-2BED-494E-9163-1FC07C6150B3}" name="Price/Pack" dataDxfId="9" dataCellStyle="Currency">
       <calculatedColumnFormula>HitsPerBox[[#This Row],[Price/Box]]/HitsPerBox[[#This Row],[Packs/Box]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D1B3B96A-22D7-9C4D-9305-A9E676F6BDD5}" name="HitPackOdds" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{0E30AA67-B526-C94B-8332-5021112F59CA}" name="Hits/box" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{D1B3B96A-22D7-9C4D-9305-A9E676F6BDD5}" name="HitPackOdds" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{0E30AA67-B526-C94B-8332-5021112F59CA}" name="Hits/box" dataDxfId="7">
       <calculatedColumnFormula>HitsPerBox[[#This Row],[Packs/Box]]/HitsPerBox[[#This Row],[HitPackOdds]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{1275F18E-C09A-1D46-AB8B-7A2E972646EF}" name="Price/Hit" dataDxfId="6" dataCellStyle="Currency">
@@ -1208,7 +1255,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1318,15 +1365,15 @@
       </c>
       <c r="E2" s="27">
         <f>_xlfn.MAXIFS(TypeOdds[JumboOdds],TypeOdds[IsHit],"Y")/SUMIF(TypeOdds[IsHit],"Y",TypeOdds[JumboNorm])</f>
-        <v>0.62935934131267601</v>
+        <v>0.62397978641717</v>
       </c>
       <c r="F2" s="23">
         <f>HitsPerBox[[#This Row],[Packs/Box]]/HitsPerBox[[#This Row],[HitPackOdds]]</f>
-        <v>15.889173868687898</v>
+        <v>16.026160170057764</v>
       </c>
       <c r="G2" s="24">
         <f>HitsPerBox[[#This Row],[Price/Box]]/HitsPerBox[[#This Row],[Hits/box]]</f>
-        <v>9.1257104490338019</v>
+        <v>9.0477069030489652</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>11</v>
@@ -1390,15 +1437,15 @@
       </c>
       <c r="E3" s="27">
         <f>_xlfn.MAXIFS(TypeOdds[HobbyOdds],TypeOdds[IsHit],"Y")/SUMIF(TypeOdds[IsHit],"Y",TypeOdds[HobbyNorm])</f>
-        <v>2.4758249411366968</v>
+        <v>2.4505452698925945</v>
       </c>
       <c r="F3" s="23">
         <f>HitsPerBox[[#This Row],[Packs/Box]]/HitsPerBox[[#This Row],[HitPackOdds]]</f>
-        <v>9.6937386812902684</v>
+        <v>9.793738681290268</v>
       </c>
       <c r="G3" s="24">
         <f>HitsPerBox[[#This Row],[Price/Box]]/HitsPerBox[[#This Row],[Hits/box]]</f>
-        <v>9.8001403919994257</v>
+        <v>9.700075026658185</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>6</v>
@@ -1454,23 +1501,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" s="17">
         <f>HitsPerBox[[#This Row],[Price/Box]]/HitsPerBox[[#This Row],[Packs/Box]]</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" s="27">
         <f>_xlfn.MAXIFS(TypeOdds[HangerOdds],TypeOdds[IsHit],"Y")/SUMIF(TypeOdds[IsHit],"Y",TypeOdds[HangerNorm])</f>
-        <v>1.1536341590807022</v>
+        <v>1.1276170090800002</v>
       </c>
       <c r="F4" s="23">
         <f>HitsPerBox[[#This Row],[Packs/Box]]/HitsPerBox[[#This Row],[HitPackOdds]]</f>
-        <v>0.8668259275513055</v>
+        <v>0.88682592755130552</v>
       </c>
       <c r="G4" s="24">
         <f>HitsPerBox[[#This Row],[Price/Box]]/HitsPerBox[[#This Row],[Hits/box]]</f>
-        <v>17.304512386210533</v>
+        <v>11.276170090800001</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>6</v>
@@ -1534,15 +1581,15 @@
       </c>
       <c r="E5" s="27">
         <f>_xlfn.MAXIFS(TypeOdds[FatOdds],TypeOdds[IsHit],"Y")/SUMIF(TypeOdds[IsHit],"Y",TypeOdds[FatNorm])</f>
-        <v>2.2726506546066005</v>
+        <v>2.2216503009622683</v>
       </c>
       <c r="F5" s="23">
         <f>HitsPerBox[[#This Row],[Packs/Box]]/HitsPerBox[[#This Row],[HitPackOdds]]</f>
-        <v>0.44001483376823775</v>
+        <v>0.45011584386924791</v>
       </c>
       <c r="G5" s="24">
         <f>HitsPerBox[[#This Row],[Price/Box]]/HitsPerBox[[#This Row],[Hits/box]]</f>
-        <v>18.181205236852804</v>
+        <v>17.773202407698147</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>6</v>
@@ -1608,15 +1655,15 @@
       </c>
       <c r="E6" s="27">
         <f>_xlfn.MAXIFS(TypeOdds[BlasterOdds],TypeOdds[IsHit],"Y")/SUMIF(TypeOdds[IsHit],"Y",TypeOdds[BlasterNorm])</f>
-        <v>4.976550064082943</v>
+        <v>4.8754544672437943</v>
       </c>
       <c r="F6" s="23">
         <f>HitsPerBox[[#This Row],[Packs/Box]]/HitsPerBox[[#This Row],[HitPackOdds]]</f>
-        <v>1.4065969215342213</v>
+        <v>1.4357635882008883</v>
       </c>
       <c r="G6" s="24">
         <f>HitsPerBox[[#This Row],[Price/Box]]/HitsPerBox[[#This Row],[Hits/box]]</f>
-        <v>14.218714468808409</v>
+        <v>13.92986990641084</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>6</v>
@@ -3620,46 +3667,48 @@
         <v>0</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L48" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="L48" s="8">
+        <v>2019</v>
+      </c>
       <c r="M48" s="13">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="N48" s="13">
-        <v>240</v>
+        <v>8</v>
       </c>
       <c r="O48" s="14">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="P48" s="14">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="Q48" s="14">
-        <v>240</v>
+        <v>8</v>
       </c>
       <c r="R48" s="18">
         <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[JumboOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[JumboOdds]],0),0)</f>
-        <v>0</v>
+        <v>26461.333333333332</v>
       </c>
       <c r="S48" s="18">
         <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HobbyOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HobbyOdds]],0),0)</f>
-        <v>0</v>
+        <v>51423</v>
       </c>
       <c r="T48" s="19">
         <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HangerOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HangerOdds]],0),0)</f>
-        <v>0</v>
+        <v>18011</v>
       </c>
       <c r="U48" s="19">
         <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[FatOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[FatOdds]],0),0)</f>
-        <v>0</v>
+        <v>21996</v>
       </c>
       <c r="V48" s="19">
         <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[BlasterOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[BlasterOdds]],0),0)</f>
-        <v>0</v>
+        <v>30661.125</v>
       </c>
     </row>
     <row r="49" spans="5:22" x14ac:dyDescent="0.15">
@@ -3668,48 +3717,48 @@
         <v>0</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>46</v>
       </c>
       <c r="L49" s="8">
-        <v>2019</v>
+        <v>150</v>
       </c>
       <c r="M49" s="13">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="N49" s="13">
-        <v>8</v>
+        <v>240</v>
       </c>
       <c r="O49" s="14">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="P49" s="14">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="Q49" s="14">
-        <v>8</v>
-      </c>
-      <c r="R49" s="18">
-        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[JumboOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[JumboOdds]],0),0)</f>
-        <v>26461.333333333332</v>
-      </c>
-      <c r="S49" s="18">
-        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HobbyOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HobbyOdds]],0),0)</f>
-        <v>51423</v>
-      </c>
-      <c r="T49" s="19">
-        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HangerOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HangerOdds]],0),0)</f>
-        <v>18011</v>
-      </c>
-      <c r="U49" s="19">
-        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[FatOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[FatOdds]],0),0)</f>
-        <v>21996</v>
-      </c>
-      <c r="V49" s="19">
-        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[BlasterOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[BlasterOdds]],0),0)</f>
-        <v>30661.125</v>
+        <v>240</v>
+      </c>
+      <c r="R49" s="31">
+        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[JumboOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[JumboOdds]],0),0)</f>
+        <v>1087.4520547945206</v>
+      </c>
+      <c r="S49" s="31">
+        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HobbyOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HobbyOdds]],0),0)</f>
+        <v>1714.1</v>
+      </c>
+      <c r="T49" s="32">
+        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[HangerOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[HangerOdds]],0),0)</f>
+        <v>720.44</v>
+      </c>
+      <c r="U49" s="32">
+        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[FatOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[FatOdds]],0),0)</f>
+        <v>888.72727272727275</v>
+      </c>
+      <c r="V49" s="32">
+        <f>IF(TypeOdds[[#This Row],[IsHit]]="Y",IFERROR(_xlfn.MAXIFS(TypeOdds[BlasterOdds],TypeOdds[IsHit],"Y")/TypeOdds[[#This Row],[BlasterOdds]],0),0)</f>
+        <v>1022.0375</v>
       </c>
     </row>
     <row r="50" spans="5:22" x14ac:dyDescent="0.15">
@@ -5973,12 +6022,28 @@
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="I2:V96">
-    <cfRule type="expression" dxfId="2" priority="5">
+  <conditionalFormatting sqref="I51:V96 I2:V47 I49:V49">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$I2&lt;&gt;$I1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$K2="N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50:V50">
+    <cfRule type="expression" dxfId="3" priority="9">
+      <formula>$I50&lt;&gt;$I48</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="10">
+      <formula>$K50="N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48:V48">
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>$I48&lt;&gt;#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>$K48="N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>